<commit_message>
add newest files to database course
</commit_message>
<xml_diff>
--- a/Tietokannat -kurssi cd_tietokanta/Tietokanta_atribuutit.xlsx
+++ b/Tietokannat -kurssi cd_tietokanta/Tietokanta_atribuutit.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\H3298\Repos\Database-Practise\Misc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\storage\homes\H3298\Dox\Desktop\Tietokannat -kurssi cd_tietokanta\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="CD" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="42">
   <si>
     <t>Nimi</t>
   </si>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>Kuvapath</t>
+  </si>
+  <si>
+    <t>Numero</t>
+  </si>
+  <si>
+    <t>Kappaleen järjestys levyllä</t>
   </si>
 </sst>
 </file>
@@ -482,7 +488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -1140,10 +1146,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1271,6 +1277,23 @@
       </c>
       <c r="F7">
         <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>